<commit_message>
new files for duration of storage incubations plus updates to t1 fluxes for arc samples and Rmd updates
</commit_message>
<xml_diff>
--- a/data/raw/lab_jena_results-co2_2018-07-30/ArcInc_IncData_2018.xlsx
+++ b/data/raw/lab_jena_results-co2_2018-07-30/ArcInc_IncData_2018.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="0" windowWidth="29960" windowHeight="19520"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="jar_information" sheetId="4" r:id="rId1"/>
@@ -1185,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="W10" sqref="W10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1485,7 +1485,7 @@
         <v>10.650786699257674</v>
       </c>
       <c r="U3" s="57">
-        <f>T3/I3</f>
+        <f t="shared" ref="U3:U16" si="1">T3/I3</f>
         <v>1.0567905557689244E-2</v>
       </c>
       <c r="V3" s="56">
@@ -1584,7 +1584,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I4" s="30">
-        <f t="shared" ref="I4:I26" si="1">((E4*H4)/(G4-E4))</f>
+        <f t="shared" ref="I4:I26" si="2">((E4*H4)/(G4-E4))</f>
         <v>979.7904191616766</v>
       </c>
       <c r="J4" s="8">
@@ -1608,7 +1608,7 @@
         <v>26.611591631551708</v>
       </c>
       <c r="R4" s="46">
-        <f t="shared" ref="R4:R22" si="2">Q4/2</f>
+        <f t="shared" ref="R4:R22" si="3">Q4/2</f>
         <v>13.305795815775854</v>
       </c>
       <c r="S4" s="55">
@@ -1619,7 +1619,7 @@
         <v>10.650786699257674</v>
       </c>
       <c r="U4" s="57">
-        <f>T4/I4</f>
+        <f t="shared" si="1"/>
         <v>1.0870474431022348E-2</v>
       </c>
       <c r="V4" s="56">
@@ -1718,7 +1718,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I5" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1007.8427216363732</v>
       </c>
       <c r="J5" s="8">
@@ -1741,7 +1741,7 @@
         <v>27.373506019753343</v>
       </c>
       <c r="R5" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.686753009876671</v>
       </c>
       <c r="S5" s="55">
@@ -1752,7 +1752,7 @@
         <v>10.650786699257674</v>
       </c>
       <c r="U5" s="57">
-        <f>T5/I5</f>
+        <f t="shared" si="1"/>
         <v>1.0567905557689236E-2</v>
       </c>
       <c r="V5" s="56">
@@ -1847,7 +1847,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I6" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>979.7904191616766</v>
       </c>
       <c r="J6" s="8">
@@ -1870,7 +1870,7 @@
         <v>26.611591631551708</v>
       </c>
       <c r="R6" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.305795815775854</v>
       </c>
       <c r="S6" s="55">
@@ -1881,7 +1881,7 @@
         <v>2.1002213089449566</v>
       </c>
       <c r="U6" s="57">
-        <f>T6/I6</f>
+        <f t="shared" si="1"/>
         <v>2.1435413817803379E-3</v>
       </c>
       <c r="V6" s="56">
@@ -1976,7 +1976,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I7" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>998.43694963015128</v>
       </c>
       <c r="J7" s="8">
@@ -1999,7 +1999,7 @@
         <v>27.118040607238672</v>
       </c>
       <c r="R7" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.559020303619336</v>
       </c>
       <c r="S7" s="55">
@@ -2010,7 +2010,7 @@
         <v>2.1002213089449566</v>
       </c>
       <c r="U7" s="57">
-        <f>T7/I7</f>
+        <f t="shared" si="1"/>
         <v>2.1035091997776492E-3</v>
       </c>
       <c r="V7" s="56">
@@ -2105,7 +2105,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I8" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>975.16281306001133</v>
       </c>
       <c r="J8" s="8">
@@ -2128,7 +2128,7 @@
         <v>26.485903564592896</v>
       </c>
       <c r="R8" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.242951782296448</v>
       </c>
       <c r="S8" s="55">
@@ -2139,7 +2139,7 @@
         <v>2.1002213089449566</v>
       </c>
       <c r="U8" s="57">
-        <f>T8/I8</f>
+        <f t="shared" si="1"/>
         <v>2.1537134936006931E-3</v>
       </c>
       <c r="V8" s="56">
@@ -2234,7 +2234,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I9" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1012.5664476070017</v>
       </c>
       <c r="J9" s="8">
@@ -2257,7 +2257,7 @@
         <v>27.501804749819797</v>
       </c>
       <c r="R9" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.750902374909899</v>
       </c>
       <c r="S9" s="55">
@@ -2268,7 +2268,7 @@
         <v>18.813122585199586</v>
       </c>
       <c r="U9" s="57">
-        <f>T9/I9</f>
+        <f t="shared" si="1"/>
         <v>1.8579642481400246E-2</v>
       </c>
       <c r="V9" s="56">
@@ -2363,7 +2363,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I10" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>998.43694963015128</v>
       </c>
       <c r="J10" s="8">
@@ -2387,7 +2387,7 @@
         <v>27.118040607238672</v>
       </c>
       <c r="R10" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.559020303619336</v>
       </c>
       <c r="S10" s="55">
@@ -2398,7 +2398,7 @@
         <v>18.813122585199586</v>
       </c>
       <c r="U10" s="57">
-        <f>T10/I10</f>
+        <f t="shared" si="1"/>
         <v>1.8842574478206649E-2</v>
       </c>
       <c r="V10" s="56">
@@ -2497,7 +2497,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I11" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1003.1329094388542</v>
       </c>
       <c r="J11" s="8">
@@ -2521,7 +2521,7 @@
         <v>27.245585194635542</v>
       </c>
       <c r="R11" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.622792597317771</v>
       </c>
       <c r="S11" s="55">
@@ -2532,7 +2532,7 @@
         <v>18.813122585199586</v>
       </c>
       <c r="U11" s="57">
-        <f>T11/I11</f>
+        <f t="shared" si="1"/>
         <v>1.8754366852268379E-2</v>
       </c>
       <c r="V11" s="56">
@@ -2631,7 +2631,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I12" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>975.16281306001133</v>
       </c>
       <c r="J12" s="8">
@@ -2654,7 +2654,7 @@
         <v>26.485903564592896</v>
       </c>
       <c r="R12" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.242951782296448</v>
       </c>
       <c r="S12" s="55">
@@ -2665,7 +2665,7 @@
         <v>3.7324844392034473</v>
       </c>
       <c r="U12" s="57">
-        <f>T12/I12</f>
+        <f t="shared" si="1"/>
         <v>3.8275500144341035E-3</v>
       </c>
       <c r="V12" s="56">
@@ -2755,7 +2755,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I13" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>975.16281306001133</v>
       </c>
       <c r="J13" s="8">
@@ -2779,7 +2779,7 @@
         <v>26.485903564592896</v>
       </c>
       <c r="R13" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.242951782296448</v>
       </c>
       <c r="S13" s="55">
@@ -2790,7 +2790,7 @@
         <v>3.7324844392034473</v>
       </c>
       <c r="U13" s="57">
-        <f>T13/I13</f>
+        <f t="shared" si="1"/>
         <v>3.8275500144341035E-3</v>
       </c>
       <c r="V13" s="56">
@@ -2889,7 +2889,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I14" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>979.7904191616766</v>
       </c>
       <c r="J14" s="8">
@@ -2913,7 +2913,7 @@
         <v>26.611591631551708</v>
       </c>
       <c r="R14" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.305795815775854</v>
       </c>
       <c r="S14" s="55">
@@ -2924,7 +2924,7 @@
         <v>3.7324844392034473</v>
       </c>
       <c r="U14" s="57">
-        <f>T14/I14</f>
+        <f t="shared" si="1"/>
         <v>3.8094722771396532E-3</v>
       </c>
       <c r="V14" s="56">
@@ -3023,7 +3023,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I15" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1007.5846827055947</v>
       </c>
       <c r="J15" s="8">
@@ -3046,7 +3046,7 @@
         <v>27.366497554966767</v>
       </c>
       <c r="R15" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.683248777483383</v>
       </c>
       <c r="S15" s="55">
@@ -3057,7 +3057,7 @@
         <v>7.2089513781016725</v>
       </c>
       <c r="U15" s="57">
-        <f>T15/I15</f>
+        <f t="shared" si="1"/>
         <v>7.1546853597893069E-3</v>
       </c>
       <c r="V15" s="56">
@@ -3147,7 +3147,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I16" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>988.77465656921436</v>
       </c>
       <c r="J16" s="8">
@@ -3170,7 +3170,7 @@
         <v>26.855607956200881</v>
       </c>
       <c r="R16" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.427803978100441</v>
       </c>
       <c r="S16" s="55">
@@ -3181,7 +3181,7 @@
         <v>9.694929332799763</v>
       </c>
       <c r="U16" s="57">
-        <f>T16/I16</f>
+        <f t="shared" si="1"/>
         <v>9.8049937550367585E-3</v>
       </c>
       <c r="V16" s="56">
@@ -3271,7 +3271,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I17" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>998.15192623602354</v>
       </c>
       <c r="J17" s="8">
@@ -3295,7 +3295,7 @@
         <v>27.110299231101873</v>
       </c>
       <c r="R17" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.555149615550937</v>
       </c>
       <c r="S17" s="61" t="s">
@@ -3387,7 +3387,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I18" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>993.45638619667875</v>
       </c>
       <c r="J18" s="8">
@@ -3411,7 +3411,7 @@
         <v>26.982766044848059</v>
       </c>
       <c r="R18" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.49138302242403</v>
       </c>
       <c r="S18" s="61" t="s">
@@ -3503,7 +3503,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I19" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>998.15192623602354</v>
       </c>
       <c r="J19" s="8">
@@ -3527,7 +3527,7 @@
         <v>27.110299231101873</v>
       </c>
       <c r="R19" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.555149615550937</v>
       </c>
       <c r="S19" s="61" t="s">
@@ -3628,7 +3628,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I20" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1007.5846827055947</v>
       </c>
       <c r="J20" s="8">
@@ -3652,7 +3652,7 @@
         <v>27.366497554966767</v>
       </c>
       <c r="R20" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.683248777483383</v>
       </c>
       <c r="S20" s="61" t="s">
@@ -3753,7 +3753,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I21" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1021.8389372814548</v>
       </c>
       <c r="J21" s="8">
@@ -3777,7 +3777,7 @@
         <v>27.753650148385191</v>
       </c>
       <c r="R21" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.876825074192595</v>
       </c>
       <c r="S21" s="61" t="s">
@@ -3863,7 +3863,7 @@
         <v>2190.1197604790418</v>
       </c>
       <c r="I22" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>998.15192623602354</v>
       </c>
       <c r="J22" s="8">
@@ -3887,7 +3887,7 @@
         <v>27.110299231101873</v>
       </c>
       <c r="R22" s="46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.555149615550937</v>
       </c>
       <c r="S22" s="61" t="s">
@@ -4022,7 +4022,7 @@
       <c r="G24" s="8"/>
       <c r="H24" s="38"/>
       <c r="I24" s="30" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J24" s="8"/>
@@ -4031,7 +4031,7 @@
         <v>1100</v>
       </c>
       <c r="M24" s="33" t="e">
-        <f t="shared" ref="M24:M26" si="3">((L24*G24)/J24)-L24</f>
+        <f t="shared" ref="M24:M26" si="4">((L24*G24)/J24)-L24</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N24" s="39"/>
@@ -4104,7 +4104,7 @@
       <c r="G25" s="8"/>
       <c r="H25" s="38"/>
       <c r="I25" s="30" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J25" s="8"/>
@@ -4113,7 +4113,7 @@
         <v>1100</v>
       </c>
       <c r="M25" s="33" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N25" s="39"/>
@@ -4186,7 +4186,7 @@
       <c r="G26" s="8"/>
       <c r="H26" s="38"/>
       <c r="I26" s="30" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="J26" s="8"/>
@@ -4195,7 +4195,7 @@
         <v>1100</v>
       </c>
       <c r="M26" s="33" t="e">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N26" s="39"/>
@@ -4215,7 +4215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>

</xml_diff>